<commit_message>
Fixed the currency symbols
The currency symbols were not showing up correctly
due to wrong formatting. Changed the formatting to UTF-8
and it worked. Not all of the symbols show, but for the
most part it's ok.

-add currency_symbols file in UTF-8 formatting
-reformat the code to use the file currency symbols
</commit_message>
<xml_diff>
--- a/BudgetPlanner implementation process.xlsx
+++ b/BudgetPlanner implementation process.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mymi.KYIV\Google Drive\coding\Android\myApps\BudgetPlanner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\android\BudgetControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="126">
   <si>
     <t>pocket budget</t>
   </si>
@@ -271,12 +271,6 @@
     <t xml:space="preserve">implement the button that  will take you to the list of available currencies. </t>
   </si>
   <si>
-    <t xml:space="preserve">The search should implement a helper.  </t>
-  </si>
-  <si>
-    <t>Once the currency is chosen it should take the user back to the budgetSettings activity with the result saved in the currency textview.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Currency field should be static. </t>
   </si>
   <si>
@@ -316,9 +310,6 @@
     <t>create a standard listview to display the currency objects on the device</t>
   </si>
   <si>
-    <t>Create a custom listview using the array of currency classes using startActivityforresult and saving the needed key value pair that will be available for later access through the app</t>
-  </si>
-  <si>
     <t>implementation of the expense page</t>
   </si>
   <si>
@@ -346,9 +337,6 @@
     <t>Making the design pretty for the statistics Page</t>
   </si>
   <si>
-    <t>make the unicode symbols show up in the UI</t>
-  </si>
-  <si>
     <t>implement the bar graph for the month</t>
   </si>
   <si>
@@ -403,7 +391,22 @@
     <t>add this file to git</t>
   </si>
   <si>
-    <t>4 hours +</t>
+    <t>the listview should implement a search</t>
+  </si>
+  <si>
+    <t>Once the currency is chosen it should take the user back to the budgetSettings activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save the currency chosen in a key-value pair </t>
+  </si>
+  <si>
+    <t>make the unicode symbols show up in the UI (try different encodings)</t>
+  </si>
+  <si>
+    <t>Sun 6pm - tues 11 am (5 hours)</t>
+  </si>
+  <si>
+    <t>5 min</t>
   </si>
 </sst>
 </file>
@@ -1549,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,7 +1576,7 @@
     <col min="16" max="16" width="23.7109375" customWidth="1"/>
     <col min="17" max="17" width="27.140625" customWidth="1"/>
     <col min="18" max="18" width="22.85546875" customWidth="1"/>
-    <col min="19" max="19" width="20.42578125" customWidth="1"/>
+    <col min="19" max="19" width="29" customWidth="1"/>
     <col min="20" max="20" width="16.7109375" customWidth="1"/>
     <col min="21" max="21" width="24" customWidth="1"/>
     <col min="22" max="22" width="18.7109375" customWidth="1"/>
@@ -1582,7 +1585,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -1604,7 +1607,7 @@
     </row>
     <row r="2" spans="1:24" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>43</v>
@@ -1625,7 +1628,7 @@
     </row>
     <row r="3" spans="1:24" ht="137.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>56</v>
@@ -1671,81 +1674,81 @@
     </row>
     <row r="5" spans="1:24" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="H5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="J5" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="K5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q5" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="Q5" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>80</v>
+      <c r="T5" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="V5" s="4" t="s">
-        <v>76</v>
+        <v>121</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>75</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="4"/>
@@ -1763,25 +1766,27 @@
       <c r="Q6" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="R6" s="1"/>
+      <c r="R6" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="S6" s="4"/>
       <c r="T6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>46</v>
@@ -1790,12 +1795,12 @@
         <v>75</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1805,10 +1810,10 @@
     </row>
     <row r="9" spans="1:24" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -1826,44 +1831,44 @@
         <v>75</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>51</v>
@@ -1871,19 +1876,19 @@
     </row>
     <row r="15" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" ht="114.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1990,7 +1995,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2067,7 +2072,7 @@
     </row>
     <row r="25" spans="2:2" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make custom currency listview
I made a custom currency listview in order to
show the currency names on the left and currency
symbols on the right.

- create a custom a layout for currency listview
- create a custom adapter for currency views
</commit_message>
<xml_diff>
--- a/BudgetPlanner implementation process.xlsx
+++ b/BudgetPlanner implementation process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="127">
   <si>
     <t>pocket budget</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>5 min</t>
+  </si>
+  <si>
+    <t>implement a custom listview for currencies</t>
   </si>
 </sst>
 </file>
@@ -1550,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X28"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1586,7 @@
     <col min="23" max="23" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1605,7 +1608,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:24" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>93</v>
       </c>
@@ -1626,7 +1629,7 @@
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:24" ht="137.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="137.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>94</v>
       </c>
@@ -1658,7 +1661,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>66</v>
       </c>
@@ -1672,7 +1675,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -1727,26 +1730,29 @@
       <c r="R5" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="U5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>95</v>
       </c>
@@ -1772,7 +1778,7 @@
       <c r="S6" s="4"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:24" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>95</v>
       </c>
@@ -1808,7 +1814,7 @@
       <c r="F8" s="11"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:24" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -1834,7 +1840,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>111</v>
       </c>
@@ -1842,7 +1848,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -1850,7 +1856,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>114</v>
       </c>
@@ -1858,7 +1864,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>115</v>
       </c>
@@ -1866,7 +1872,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>116</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
added a new task
</commit_message>
<xml_diff>
--- a/BudgetPlanner implementation process.xlsx
+++ b/BudgetPlanner implementation process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="129">
   <si>
     <t>pocket budget</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t>implement a custom listview for currencies</t>
+  </si>
+  <si>
+    <t>delete the currency class and other stuff if it's not needed</t>
+  </si>
+  <si>
+    <t>2.5 hours</t>
   </si>
 </sst>
 </file>
@@ -1553,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y28"/>
+  <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" topLeftCell="Q4" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,10 +1589,10 @@
     <col min="20" max="20" width="16.7109375" customWidth="1"/>
     <col min="21" max="21" width="24" customWidth="1"/>
     <col min="22" max="22" width="18.7109375" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" customWidth="1"/>
+    <col min="23" max="23" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1608,7 +1614,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>93</v>
       </c>
@@ -1629,7 +1635,7 @@
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:25" ht="137.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="137.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>94</v>
       </c>
@@ -1661,7 +1667,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>66</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -1730,7 +1736,7 @@
       <c r="R5" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="S5" s="7" t="s">
         <v>126</v>
       </c>
       <c r="T5" s="1" t="s">
@@ -1739,20 +1745,23 @@
       <c r="U5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>95</v>
       </c>
@@ -1775,10 +1784,12 @@
       <c r="R6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="S6" s="4"/>
+      <c r="S6" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:25" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -1804,7 +1815,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>95</v>
       </c>
@@ -1814,7 +1825,7 @@
       <c r="F8" s="11"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:25" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -1840,7 +1851,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>111</v>
       </c>
@@ -1848,7 +1859,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -1856,7 +1867,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>114</v>
       </c>
@@ -1864,7 +1875,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>115</v>
       </c>
@@ -1872,7 +1883,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>116</v>
       </c>
@@ -1880,7 +1891,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
Add onClickListener to CurrencyActivity
I added an onclick listener to CurrencyListActivity
and saved the currency that the used chose in a
currencyUsed variable for later access in other classes
and activities. The currency chosen should prepend
every money variable in the app.

- Added onclick listener to the listView
- Saved the chosen currency in a currencyUsed variable
for later access
</commit_message>
<xml_diff>
--- a/BudgetPlanner implementation process.xlsx
+++ b/BudgetPlanner implementation process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="130">
   <si>
     <t>pocket budget</t>
   </si>
@@ -259,9 +259,6 @@
     <t>write JavaDoc and comments</t>
   </si>
   <si>
-    <t xml:space="preserve">apply currency to everything once it is implemented. </t>
-  </si>
-  <si>
     <t>implement the currency textview in the budget settings activity</t>
   </si>
   <si>
@@ -397,9 +394,6 @@
     <t>Once the currency is chosen it should take the user back to the budgetSettings activity</t>
   </si>
   <si>
-    <t xml:space="preserve">save the currency chosen in a key-value pair </t>
-  </si>
-  <si>
     <t>make the unicode symbols show up in the UI (try different encodings)</t>
   </si>
   <si>
@@ -416,6 +410,15 @@
   </si>
   <si>
     <t>2.5 hours</t>
+  </si>
+  <si>
+    <t>apply currency to everything once it is implemented. (See how other projects are doing this)</t>
+  </si>
+  <si>
+    <t>save the currency chosen in a key-value pair or a variable</t>
+  </si>
+  <si>
+    <t>25-06-2014  10:30:00 AM - 4 PM June 26th (2 - 3 hours)</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -525,6 +528,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1562,7 +1568,7 @@
   <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q4" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1600,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -1616,7 +1622,7 @@
     </row>
     <row r="2" spans="1:26" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>43</v>
@@ -1637,7 +1643,7 @@
     </row>
     <row r="3" spans="1:26" ht="137.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>56</v>
@@ -1683,87 +1689,87 @@
     </row>
     <row r="5" spans="1:26" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="L5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="M5" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="O5" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X5" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="V5" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>75</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="4"/>
@@ -1779,31 +1785,33 @@
       <c r="N6" s="9"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="T6" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>46</v>
@@ -1812,12 +1820,12 @@
         <v>75</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1827,10 +1835,10 @@
     </row>
     <row r="9" spans="1:26" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -1848,44 +1856,44 @@
         <v>75</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>51</v>
@@ -1893,19 +1901,19 @@
     </row>
     <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" ht="114.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2000,19 +2008,19 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2084,12 +2092,12 @@
     </row>
     <row r="24" spans="2:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put the chosen currency into sharedPreferences
The chosen currency before was put into a
static variable in CurrencyList class. Right now
the currency will be saved into a key-value pair
for later access in other activites.

-add sharedPreferences to CurrencyListActivity
-save the chosen currency in a key-value pair
</commit_message>
<xml_diff>
--- a/BudgetPlanner implementation process.xlsx
+++ b/BudgetPlanner implementation process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="131">
   <si>
     <t>pocket budget</t>
   </si>
@@ -419,6 +419,9 @@
   </si>
   <si>
     <t>25-06-2014  10:30:00 AM - 4 PM June 26th (2 - 3 hours)</t>
+  </si>
+  <si>
+    <t>ask Borys Pratsiuk what else do I need to study to qualify for a Junior Android Developer</t>
   </si>
 </sst>
 </file>
@@ -1567,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,10 +1764,10 @@
         <v>119</v>
       </c>
       <c r="Y5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z5" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1914,6 +1917,11 @@
       </c>
       <c r="E15" s="2" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="28" ht="114.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>